<commit_message>
Updated parts list for the gantry
</commit_message>
<xml_diff>
--- a/Parts List/Gantry_Parts_List.xlsx
+++ b/Parts List/Gantry_Parts_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tankh\Documents\3D Modeling\CNC Laser\Laser Cutter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tankh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Item</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>20mm x 80mm, 1000mm, Silver</t>
+  </si>
+  <si>
+    <t>http://openbuildspartstore.com/90-degree-joining-plate/</t>
+  </si>
+  <si>
+    <t>90 Degree Joining Plate</t>
+  </si>
+  <si>
+    <t>Connect X axis to Y axis</t>
+  </si>
+  <si>
+    <t>1500mm, Silver</t>
+  </si>
+  <si>
+    <t>u.;</t>
   </si>
 </sst>
 </file>
@@ -522,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +588,7 @@
         <v>139.94999999999999</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F10" si="0">D2*E2</f>
+        <f t="shared" ref="F2:F13" si="0">D2*E2</f>
         <v>419.84999999999997</v>
       </c>
     </row>
@@ -745,10 +760,57 @@
         <v>47.95</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>23</v>
+      </c>
+      <c r="F11" s="3">
+        <f>D11*E11</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="F12" s="3">
+        <f>D12*E12</f>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F19" s="3">
-        <f>SUM(F2:F10)</f>
-        <v>978.75</v>
+        <f>SUM(F2:F13)</f>
+        <v>1011.35</v>
       </c>
     </row>
   </sheetData>
@@ -762,6 +824,8 @@
     <hyperlink ref="C8" r:id="rId7"/>
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the parts list to include smothie board from openbuilds
</commit_message>
<xml_diff>
--- a/Parts List/Gantry_Parts_List.xlsx
+++ b/Parts List/Gantry_Parts_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tankh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tankh\Documents\GitHub\RRCC_Laser_Lab\Parts List\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Item</t>
   </si>
@@ -89,9 +89,6 @@
     <t>http://openbuildspartstore.com/tee-nuts-25-pack/</t>
   </si>
   <si>
-    <t>Control Board</t>
-  </si>
-  <si>
     <t>Low Profile M5 Screws</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>http://openbuildspartstore.com/low-profile-screws-m5/</t>
   </si>
   <si>
-    <t>https://shop.uberclock.com/collections/smoothie/products/smoothieboard-4x</t>
-  </si>
-  <si>
     <t>Smothieboard 4x</t>
   </si>
   <si>
@@ -134,7 +128,10 @@
     <t>1500mm, Silver</t>
   </si>
   <si>
-    <t>u.;</t>
+    <t>Smoothieboard 5xC v1.1</t>
+  </si>
+  <si>
+    <t>http://openbuildspartstore.com/smoothieboard-5xc-v1-1/</t>
   </si>
 </sst>
 </file>
@@ -537,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,7 +585,7 @@
         <v>139.94999999999999</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F13" si="0">D2*E2</f>
+        <f t="shared" ref="F2:F10" si="0">D2*E2</f>
         <v>419.84999999999997</v>
       </c>
     </row>
@@ -597,7 +594,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -618,7 +615,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
@@ -699,34 +696,34 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>129.94999999999999</v>
+        <v>165.95</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
-        <v>129.94999999999999</v>
+        <v>165.95</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="D9" s="1">
         <v>4</v>
@@ -741,13 +738,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -765,7 +762,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>9</v>
@@ -783,13 +780,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -802,15 +799,10 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E15" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F19" s="3">
         <f>SUM(F2:F13)</f>
-        <v>1011.35</v>
+        <v>1047.3499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>